<commit_message>
SHIP-3 Education-changes made in the algori.
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_SHIP_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_SHIP_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981757C9-C411-4E67-A860-9320E0605D5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA854478-31FB-4B44-AB62-A5EE632F552F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="204">
   <si>
     <t>index</t>
   </si>
@@ -443,9 +443,6 @@
   </si>
   <si>
     <t>AGE</t>
-  </si>
-  <si>
-    <t>edlevel_s0</t>
   </si>
   <si>
     <t>impossible</t>
@@ -611,12 +608,6 @@
   </si>
   <si>
     <t xml:space="preserve">case_when(                                                                                                                        mi_01 %in% 1 | ang_01 %in% 1 ~ 1,                                                                                    mi_01 %in% 0 &amp; ang_01 %in% 0 ~ 0,                                                                    TRUE ~ NA_real_ )  </t>
-  </si>
-  <si>
-    <t>ang_01b_4</t>
-  </si>
-  <si>
-    <t>mi_03b5_4</t>
   </si>
   <si>
     <t>recode(0=0; 1=1; 2=3;)</t>
@@ -690,6 +681,21 @@
   </si>
   <si>
     <t>sportwi1;sportwi3;sportso1;sportso3</t>
+  </si>
+  <si>
+    <t>ang_01b</t>
+  </si>
+  <si>
+    <t>mi_03b5</t>
+  </si>
+  <si>
+    <t>proximate</t>
+  </si>
+  <si>
+    <t>case_when(                                                                               ausbild7 %in% c(1) ~ 7L,                                                        ausbild6 %in% c(1) ~ 6L,                                       ausbild5 %in% c(1) | ausbild4 %in% c(1) ~ 4L,                            Schule1 %in% c(7,8) ~ 3L,                                              Schule1 %in% c(3,4,5,6) ~ 2L,                               Schule1 %in% c(2) ~ 0L,                                                  ausbild8 %in% c(1) | ausbild %in% c(1) | Schule1 %in% c(1,9) ~ 9L,                                                                       TRUE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>ausbild7 ;ausbild6 ; ausbild5;Schule1; ausbild8;ausbild; ausbild4</t>
   </si>
 </sst>
 </file>
@@ -785,7 +791,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -837,6 +843,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1179,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,7 +1324,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="4" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
@@ -1325,20 +1334,20 @@
       <c r="D5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>178</v>
+      <c r="F5" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>202</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>178</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1352,19 +1361,19 @@
         <v>18</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1378,19 +1387,19 @@
         <v>13</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>136</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="165" x14ac:dyDescent="0.25">
@@ -1404,22 +1413,22 @@
         <v>13</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>136</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1433,10 +1442,10 @@
         <v>13</v>
       </c>
       <c r="F9" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>166</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>167</v>
       </c>
       <c r="H9" s="13">
         <v>0</v>
@@ -1446,7 +1455,7 @@
         <v>136</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1460,17 +1469,17 @@
         <v>18</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I10" s="18"/>
       <c r="J10" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="K10" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1484,7 +1493,7 @@
         <v>18</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>139</v>
@@ -1511,20 +1520,20 @@
         <v>18</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I12" s="18"/>
       <c r="J12" s="5" t="s">
         <v>136</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1538,17 +1547,17 @@
         <v>18</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I13"/>
       <c r="J13" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1563,17 +1572,17 @@
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I14" s="19"/>
       <c r="J14" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="K14" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1587,19 +1596,19 @@
         <v>13</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>136</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1613,19 +1622,19 @@
         <v>13</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>136</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -1639,7 +1648,7 @@
         <v>13</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>139</v>
@@ -1666,7 +1675,7 @@
         <v>13</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>139</v>
@@ -1675,7 +1684,7 @@
         <v>139</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>137</v>
@@ -1692,16 +1701,16 @@
         <v>18</v>
       </c>
       <c r="G19" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="K19" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -1715,7 +1724,7 @@
         <v>13</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>139</v>
@@ -1742,7 +1751,7 @@
         <v>13</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>139</v>
@@ -1769,22 +1778,22 @@
         <v>13</v>
       </c>
       <c r="F22" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="H22" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="G22" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="H22" s="11" t="s">
+      <c r="I22" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="I22" s="15" t="s">
-        <v>181</v>
-      </c>
       <c r="J22" s="10" t="s">
         <v>136</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
@@ -1798,7 +1807,7 @@
         <v>13</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>139</v>
@@ -1825,22 +1834,22 @@
         <v>13</v>
       </c>
       <c r="F24" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="G24" s="5" t="s">
-        <v>171</v>
-      </c>
       <c r="H24" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>136</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="2:11" ht="120" x14ac:dyDescent="0.25">
@@ -1854,22 +1863,22 @@
         <v>13</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G25" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="H25" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="H25" s="9" t="s">
+      <c r="I25" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="I25" s="7" t="s">
-        <v>173</v>
-      </c>
       <c r="J25" s="5" t="s">
         <v>136</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="2:11" ht="135" x14ac:dyDescent="0.25">
@@ -1883,22 +1892,22 @@
         <v>13</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H26" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="I26" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="I26" s="7" t="s">
-        <v>176</v>
-      </c>
       <c r="J26" s="5" t="s">
         <v>136</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
@@ -1913,17 +1922,17 @@
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I27" s="5"/>
       <c r="J27" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
@@ -1937,7 +1946,7 @@
         <v>13</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>139</v>
@@ -1965,17 +1974,17 @@
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
@@ -1990,17 +1999,17 @@
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I30" s="5"/>
       <c r="J30" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
@@ -2015,17 +2024,17 @@
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
@@ -2040,17 +2049,17 @@
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I32" s="5"/>
       <c r="J32" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
@@ -2065,17 +2074,17 @@
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I33" s="5"/>
       <c r="J33" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
@@ -2089,7 +2098,7 @@
         <v>13</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>139</v>
@@ -2116,7 +2125,7 @@
         <v>13</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>139</v>
@@ -2143,22 +2152,22 @@
         <v>13</v>
       </c>
       <c r="F36" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="H36" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="G36" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="H36" s="15" t="s">
-        <v>191</v>
-      </c>
       <c r="I36" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J36" s="10" t="s">
         <v>136</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="2:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2172,7 +2181,7 @@
         <v>18</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>139</v>
@@ -2198,16 +2207,16 @@
         <v>13</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K38" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
@@ -2221,7 +2230,7 @@
         <v>18</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>139</v>
@@ -2248,7 +2257,7 @@
         <v>13</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>139</v>
@@ -2275,16 +2284,16 @@
         <v>18</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
@@ -2298,7 +2307,7 @@
         <v>13</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>139</v>
@@ -2326,16 +2335,16 @@
       </c>
       <c r="F43" s="11"/>
       <c r="G43" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K43" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
@@ -2350,19 +2359,19 @@
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2376,19 +2385,19 @@
         <v>18</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I45" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
@@ -2403,19 +2412,19 @@
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
@@ -2430,19 +2439,19 @@
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
@@ -2457,19 +2466,19 @@
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
@@ -2484,19 +2493,19 @@
       </c>
       <c r="F49" s="5"/>
       <c r="G49" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
@@ -2510,7 +2519,7 @@
         <v>13</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>139</v>
@@ -2537,19 +2546,19 @@
         <v>18</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I51" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
@@ -2563,7 +2572,7 @@
         <v>13</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>139</v>
@@ -2590,16 +2599,16 @@
         <v>18</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
@@ -2613,7 +2622,7 @@
         <v>13</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>139</v>
@@ -2641,16 +2650,16 @@
       </c>
       <c r="F55" s="17"/>
       <c r="G55" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="56" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2665,16 +2674,16 @@
       </c>
       <c r="F56" s="17"/>
       <c r="G56" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2688,7 +2697,7 @@
         <v>13</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>139</v>
@@ -2714,7 +2723,7 @@
         <v>18</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>139</v>
@@ -2740,7 +2749,7 @@
         <v>13</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>139</v>
@@ -2767,7 +2776,7 @@
         <v>13</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>139</v>
@@ -2794,20 +2803,20 @@
         <v>18</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I61" s="5"/>
       <c r="J61" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>